<commit_message>
good on unseen but bad on test?
</commit_message>
<xml_diff>
--- a/results/traditional_model_results.xlsx
+++ b/results/traditional_model_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,22 +441,33 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sensitivity (w/o resampling)</t>
+          <t>Sensitivity</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Specificity (w/o resampling)</t>
+          <t>Specificity</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>F1-score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Sensitivity (w/ resampling)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Specificity (w/ resampling)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>F1-Score (w/ resampling)</t>
         </is>
       </c>
     </row>
@@ -476,10 +487,17 @@
         <v>84.96644295302013</v>
       </c>
       <c r="E2" t="n">
+        <v>0.8288832234665614</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
         <v>84.09999999999999</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>84.3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8418941199624707</v>
       </c>
     </row>
     <row r="3">
@@ -498,10 +516,17 @@
         <v>84.6979865771812</v>
       </c>
       <c r="E3" t="n">
+        <v>0.8350927033463117</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
         <v>99.2</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>95.8</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9749928291636436</v>
       </c>
     </row>
     <row r="4">
@@ -510,7 +535,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LogR</t>
+          <t>LogitR</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -520,10 +545,17 @@
         <v>78.38926174496645</v>
       </c>
       <c r="E4" t="n">
+        <v>0.7979078887464386</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
         <v>67.2</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>80.59999999999999</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.7375805834715173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>